<commit_message>
fix multiple eel spawns on search
</commit_message>
<xml_diff>
--- a/MG.xlsx
+++ b/MG.xlsx
@@ -58,7 +58,7 @@
     <t>P20199</t>
   </si>
   <si>
-    <t>P20204</t>
+    <t>P83637</t>
   </si>
 </sst>
 </file>
@@ -77,7 +77,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>

</xml_diff>